<commit_message>
Update project03 - 요구사항 정의서 - 서희.xlsx
</commit_message>
<xml_diff>
--- a/project03 - 요구사항 정의서 - 서희.xlsx
+++ b/project03 - 요구사항 정의서 - 서희.xlsx
@@ -604,14 +604,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>프로젝트 제작 회원 (메이커)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 투자 회원 (서포터)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자 로그인</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -674,11 +666,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>입출금 및 투자내역 관리, 예치금 관리(몰수/부여/사용제한 등). 투자 제한(간단한 사유 포함), 강제 탈퇴
-(탈퇴한 회원은 회색 음영 표시)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>프로젝트 소개 페이지 연결, 업체 연락처, 펀딩 페이지 열기 제한/해제, 강제 탈퇴
  (탈퇴한 회원은 회색 음영 표시)</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -697,11 +684,6 @@
   </si>
   <si>
     <t>상단 고정 공지사항 선택, 등록/수정/삭제</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 별 결제 현황, 결제 진행
-(펀딩성공-결제대기/펀딩성공-결제완료/펀딩실패-락업해제대기/펀딩성공-락업해제완료)</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -872,6 +854,24 @@
   </si>
   <si>
     <t>기범</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 제작 회원 (메이커)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 투자 회원 (서포터)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>입출금 및 투자내역 관리, 예치금 관리(몰수/부여/사용제한 등). 투자 제한(간단한 사유 포함), 강제 탈퇴
+(탈퇴한 회원은 회색 음영 표시)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 별 결제 현황, 결제 진행
+(펀딩성공-결제대기/펀딩성공-결제완료/펀딩실패-락업해제대기/펀딩실패-락업해제완료)</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1659,6 +1659,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1736,33 +1763,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1981,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2040,22 +2040,22 @@
     </row>
     <row r="2" spans="1:33" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="85"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -2077,20 +2077,20 @@
     </row>
     <row r="3" spans="1:33" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="88"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -2238,13 +2238,13 @@
       <c r="F7" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="89" t="s">
+      <c r="G7" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
       <c r="L7" s="43" t="s">
         <v>8</v>
       </c>
@@ -2279,15 +2279,15 @@
       <c r="AG7" s="1"/>
     </row>
     <row r="8" spans="1:33" ht="33" customHeight="1">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="56" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -2326,15 +2326,15 @@
       <c r="AG8" s="1"/>
     </row>
     <row r="9" spans="1:33" ht="33" customHeight="1">
-      <c r="A9" s="73"/>
-      <c r="B9" s="80" t="s">
+      <c r="A9" s="82"/>
+      <c r="B9" s="89" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -2373,13 +2373,13 @@
       <c r="AG9" s="1"/>
     </row>
     <row r="10" spans="1:33" ht="33" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="19" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2418,13 +2418,13 @@
       <c r="AG10" s="1"/>
     </row>
     <row r="11" spans="1:33" ht="33" customHeight="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="81"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="19" t="s">
         <v>57</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2463,13 +2463,13 @@
       <c r="AG11" s="1"/>
     </row>
     <row r="12" spans="1:33" ht="33" customHeight="1">
-      <c r="A12" s="73"/>
-      <c r="B12" s="82"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="19" t="s">
         <v>81</v>
       </c>
       <c r="D12" s="58" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2502,15 +2502,15 @@
       <c r="AG12" s="1"/>
     </row>
     <row r="13" spans="1:33" ht="33" customHeight="1">
-      <c r="A13" s="73"/>
-      <c r="B13" s="93" t="s">
+      <c r="A13" s="82"/>
+      <c r="B13" s="102" t="s">
         <v>82</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="58" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2549,13 +2549,13 @@
       <c r="AG13" s="1"/>
     </row>
     <row r="14" spans="1:33" ht="33" customHeight="1">
-      <c r="A14" s="73"/>
-      <c r="B14" s="94"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2594,15 +2594,15 @@
       <c r="AG14" s="1"/>
     </row>
     <row r="15" spans="1:33" ht="33" customHeight="1">
-      <c r="A15" s="73"/>
-      <c r="B15" s="93" t="s">
+      <c r="A15" s="82"/>
+      <c r="B15" s="102" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2641,13 +2641,13 @@
       <c r="AG15" s="1"/>
     </row>
     <row r="16" spans="1:33" ht="33" customHeight="1">
-      <c r="A16" s="73"/>
-      <c r="B16" s="95"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="19" t="s">
         <v>59</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2686,13 +2686,13 @@
       <c r="AG16" s="1"/>
     </row>
     <row r="17" spans="1:33" ht="33" customHeight="1">
-      <c r="A17" s="73"/>
-      <c r="B17" s="95"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="19" t="s">
         <v>63</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2731,13 +2731,13 @@
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:33" ht="33" customHeight="1">
-      <c r="A18" s="73"/>
-      <c r="B18" s="95"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="19" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2776,13 +2776,13 @@
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:33" ht="33" customHeight="1">
-      <c r="A19" s="73"/>
-      <c r="B19" s="95"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="19" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2821,13 +2821,13 @@
       <c r="AG19" s="1"/>
     </row>
     <row r="20" spans="1:33" ht="33" customHeight="1">
-      <c r="A20" s="73"/>
-      <c r="B20" s="94"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="103"/>
       <c r="C20" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E20" s="41"/>
       <c r="F20" s="15"/>
@@ -2866,15 +2866,15 @@
       <c r="AG20" s="1"/>
     </row>
     <row r="21" spans="1:33" ht="33" customHeight="1">
-      <c r="A21" s="73"/>
-      <c r="B21" s="90" t="s">
+      <c r="A21" s="82"/>
+      <c r="B21" s="99" t="s">
         <v>84</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
@@ -2909,13 +2909,13 @@
       <c r="AG21" s="1"/>
     </row>
     <row r="22" spans="1:33" ht="33" customHeight="1">
-      <c r="A22" s="73"/>
-      <c r="B22" s="91"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="14"/>
@@ -2954,13 +2954,13 @@
       <c r="AG22" s="1"/>
     </row>
     <row r="23" spans="1:33" ht="33" customHeight="1">
-      <c r="A23" s="73"/>
-      <c r="B23" s="91"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="14"/>
@@ -2999,13 +2999,13 @@
       <c r="AG23" s="1"/>
     </row>
     <row r="24" spans="1:33" ht="33" customHeight="1">
-      <c r="A24" s="73"/>
-      <c r="B24" s="92"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="101"/>
       <c r="C24" s="42" t="s">
         <v>67</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="14"/>
@@ -3044,7 +3044,7 @@
       <c r="AG24" s="1"/>
     </row>
     <row r="25" spans="1:33" ht="33" customHeight="1" thickBot="1">
-      <c r="A25" s="74"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="28" t="s">
         <v>68</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>69</v>
       </c>
       <c r="D25" s="62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
@@ -3091,15 +3091,15 @@
       <c r="AG25" s="1"/>
     </row>
     <row r="26" spans="1:33" ht="33" customHeight="1" thickTop="1">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="79"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
@@ -3132,15 +3132,15 @@
       <c r="AG26" s="1"/>
     </row>
     <row r="27" spans="1:33" ht="33" customHeight="1">
-      <c r="A27" s="76"/>
-      <c r="B27" s="96" t="s">
+      <c r="A27" s="85"/>
+      <c r="B27" s="105" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="D27" s="64" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3177,13 +3177,13 @@
       <c r="AG27" s="1"/>
     </row>
     <row r="28" spans="1:33" ht="33" customHeight="1">
-      <c r="A28" s="76"/>
-      <c r="B28" s="96"/>
+      <c r="A28" s="85"/>
+      <c r="B28" s="105"/>
       <c r="C28" s="20" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="D28" s="65" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -3220,15 +3220,15 @@
       <c r="AG28" s="1"/>
     </row>
     <row r="29" spans="1:33" ht="33" customHeight="1">
-      <c r="A29" s="76"/>
-      <c r="B29" s="97" t="s">
+      <c r="A29" s="85"/>
+      <c r="B29" s="106" t="s">
         <v>73</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>71</v>
       </c>
       <c r="D29" s="65" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -3265,13 +3265,13 @@
       <c r="AG29" s="1"/>
     </row>
     <row r="30" spans="1:33" ht="33" customHeight="1">
-      <c r="A30" s="76"/>
-      <c r="B30" s="97"/>
+      <c r="A30" s="85"/>
+      <c r="B30" s="106"/>
       <c r="C30" s="20" t="s">
         <v>72</v>
       </c>
       <c r="D30" s="66" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
@@ -3308,7 +3308,7 @@
       <c r="AG30" s="1"/>
     </row>
     <row r="31" spans="1:33" ht="33" customHeight="1">
-      <c r="A31" s="76"/>
+      <c r="A31" s="85"/>
       <c r="B31" s="20" t="s">
         <v>74</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>79</v>
       </c>
       <c r="D31" s="66" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -3351,15 +3351,15 @@
       <c r="AG31" s="1"/>
     </row>
     <row r="32" spans="1:33" ht="33" customHeight="1">
-      <c r="A32" s="76"/>
-      <c r="B32" s="80" t="s">
-        <v>89</v>
+      <c r="A32" s="85"/>
+      <c r="B32" s="89" t="s">
+        <v>87</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>85</v>
       </c>
       <c r="D32" s="66" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -3392,13 +3392,13 @@
       <c r="AG32" s="1"/>
     </row>
     <row r="33" spans="1:33" ht="33" customHeight="1">
-      <c r="A33" s="76"/>
-      <c r="B33" s="81"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="90"/>
       <c r="C33" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D33" s="66" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -3431,13 +3431,13 @@
       <c r="AG33" s="1"/>
     </row>
     <row r="34" spans="1:33" ht="33" customHeight="1">
-      <c r="A34" s="76"/>
-      <c r="B34" s="81"/>
+      <c r="A34" s="85"/>
+      <c r="B34" s="90"/>
       <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="66" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -3470,13 +3470,13 @@
       <c r="AG34" s="1"/>
     </row>
     <row r="35" spans="1:33" ht="33" customHeight="1">
-      <c r="A35" s="76"/>
-      <c r="B35" s="82"/>
+      <c r="A35" s="85"/>
+      <c r="B35" s="91"/>
       <c r="C35" s="20" t="s">
         <v>75</v>
       </c>
       <c r="D35" s="64" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E35" s="40"/>
       <c r="F35" s="40"/>
@@ -3509,13 +3509,13 @@
       <c r="AG35" s="1"/>
     </row>
     <row r="36" spans="1:33" ht="33" customHeight="1">
-      <c r="A36" s="76"/>
-      <c r="B36" s="96" t="s">
+      <c r="A36" s="85"/>
+      <c r="B36" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="96"/>
+      <c r="C36" s="105"/>
       <c r="D36" s="64" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="E36" s="40"/>
       <c r="F36" s="40"/>
@@ -3548,13 +3548,13 @@
       <c r="AG36" s="1"/>
     </row>
     <row r="37" spans="1:33" ht="33" customHeight="1">
-      <c r="A37" s="76"/>
-      <c r="B37" s="97" t="s">
+      <c r="A37" s="85"/>
+      <c r="B37" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="97"/>
+      <c r="C37" s="106"/>
       <c r="D37" s="67" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E37" s="40"/>
       <c r="F37" s="40"/>
@@ -3587,13 +3587,13 @@
       <c r="AG37" s="1"/>
     </row>
     <row r="38" spans="1:33" ht="33" customHeight="1">
-      <c r="A38" s="77"/>
-      <c r="B38" s="97" t="s">
+      <c r="A38" s="86"/>
+      <c r="B38" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="97"/>
+      <c r="C38" s="106"/>
       <c r="D38" s="68" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
@@ -11545,22 +11545,22 @@
     </row>
     <row r="2" spans="1:33" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="85"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="94"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -11582,20 +11582,20 @@
     </row>
     <row r="3" spans="1:33" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="88"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -11743,13 +11743,13 @@
       <c r="F7" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="89" t="s">
+      <c r="G7" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
       <c r="L7" s="69" t="s">
         <v>8</v>
       </c>
@@ -11784,15 +11784,15 @@
       <c r="AG7" s="1"/>
     </row>
     <row r="8" spans="1:33" ht="33" customHeight="1">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="87" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="56" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -11831,15 +11831,15 @@
       <c r="AG8" s="1"/>
     </row>
     <row r="9" spans="1:33" ht="33" customHeight="1">
-      <c r="A9" s="73"/>
-      <c r="B9" s="80" t="s">
+      <c r="A9" s="82"/>
+      <c r="B9" s="89" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="39" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -11878,13 +11878,13 @@
       <c r="AG9" s="1"/>
     </row>
     <row r="10" spans="1:33" ht="33" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="71" t="s">
         <v>56</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -11923,13 +11923,13 @@
       <c r="AG10" s="1"/>
     </row>
     <row r="11" spans="1:33" ht="33" customHeight="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="81"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="71" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -11968,13 +11968,13 @@
       <c r="AG11" s="1"/>
     </row>
     <row r="12" spans="1:33" ht="33" customHeight="1">
-      <c r="A12" s="73"/>
-      <c r="B12" s="82"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="71" t="s">
         <v>81</v>
       </c>
       <c r="D12" s="58" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -12007,15 +12007,15 @@
       <c r="AG12" s="1"/>
     </row>
     <row r="13" spans="1:33" ht="33" customHeight="1">
-      <c r="A13" s="73"/>
-      <c r="B13" s="93" t="s">
+      <c r="A13" s="82"/>
+      <c r="B13" s="102" t="s">
         <v>82</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D13" s="58" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -12054,13 +12054,13 @@
       <c r="AG13" s="1"/>
     </row>
     <row r="14" spans="1:33" ht="42" customHeight="1">
-      <c r="A14" s="73"/>
-      <c r="B14" s="94"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="70" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -12099,15 +12099,15 @@
       <c r="AG14" s="1"/>
     </row>
     <row r="15" spans="1:33" ht="33" customHeight="1">
-      <c r="A15" s="73"/>
-      <c r="B15" s="93" t="s">
+      <c r="A15" s="82"/>
+      <c r="B15" s="102" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="70" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -12146,13 +12146,13 @@
       <c r="AG15" s="1"/>
     </row>
     <row r="16" spans="1:33" ht="33" customHeight="1">
-      <c r="A16" s="73"/>
-      <c r="B16" s="95"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="71" t="s">
         <v>59</v>
       </c>
       <c r="D16" s="58" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -12191,13 +12191,13 @@
       <c r="AG16" s="1"/>
     </row>
     <row r="17" spans="1:33" ht="33" customHeight="1">
-      <c r="A17" s="73"/>
-      <c r="B17" s="95"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="71" t="s">
         <v>63</v>
       </c>
       <c r="D17" s="58" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -12236,13 +12236,13 @@
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:33" ht="33" customHeight="1">
-      <c r="A18" s="73"/>
-      <c r="B18" s="95"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="71" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -12281,13 +12281,13 @@
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:33" ht="33" customHeight="1">
-      <c r="A19" s="73"/>
-      <c r="B19" s="95"/>
+      <c r="A19" s="82"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="71" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -12326,13 +12326,13 @@
       <c r="AG19" s="1"/>
     </row>
     <row r="20" spans="1:33" ht="33" customHeight="1">
-      <c r="A20" s="73"/>
-      <c r="B20" s="94"/>
+      <c r="A20" s="82"/>
+      <c r="B20" s="103"/>
       <c r="C20" s="70" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="60" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E20" s="41"/>
       <c r="F20" s="15"/>
@@ -12371,15 +12371,15 @@
       <c r="AG20" s="1"/>
     </row>
     <row r="21" spans="1:33" ht="33" customHeight="1">
-      <c r="A21" s="73"/>
-      <c r="B21" s="90" t="s">
-        <v>136</v>
+      <c r="A21" s="82"/>
+      <c r="B21" s="99" t="s">
+        <v>132</v>
       </c>
       <c r="C21" s="70" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="11"/>
@@ -12414,13 +12414,13 @@
       <c r="AG21" s="1"/>
     </row>
     <row r="22" spans="1:33" ht="33" customHeight="1">
-      <c r="A22" s="73"/>
-      <c r="B22" s="91"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="70" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="58" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="14"/>
@@ -12459,13 +12459,13 @@
       <c r="AG22" s="1"/>
     </row>
     <row r="23" spans="1:33" ht="33" customHeight="1">
-      <c r="A23" s="73"/>
-      <c r="B23" s="91"/>
+      <c r="A23" s="82"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="70" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D23" s="61" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="14"/>
@@ -12504,23 +12504,23 @@
       <c r="AG23" s="1"/>
     </row>
     <row r="24" spans="1:33" ht="33" customHeight="1">
-      <c r="A24" s="73"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="98" t="s">
+      <c r="A24" s="82"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="E24" s="100"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="102"/>
-      <c r="H24" s="102"/>
-      <c r="I24" s="102"/>
-      <c r="J24" s="103"/>
-      <c r="K24" s="104"/>
-      <c r="L24" s="105"/>
-      <c r="M24" s="106"/>
+      <c r="D24" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="74"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="80"/>
       <c r="N24" s="8">
         <v>1</v>
       </c>
@@ -12549,15 +12549,15 @@
       <c r="AG24" s="1"/>
     </row>
     <row r="25" spans="1:33" ht="33" customHeight="1" thickBot="1">
-      <c r="A25" s="74"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="71" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C25" s="71" t="s">
         <v>69</v>
       </c>
       <c r="D25" s="66" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E25" s="71"/>
       <c r="F25" s="71"/>
@@ -12875,7 +12875,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="2"/>

</xml_diff>